<commit_message>
convertir a csv a excel
</commit_message>
<xml_diff>
--- a/temp/archivo.xlsx
+++ b/temp/archivo.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="hoja2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +444,16 @@
           <t>State</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Postal</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Population</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -455,6 +464,14 @@
           <t>Alabama</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4849377</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -465,6 +482,14 @@
           <t>Alaska</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>736732</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -475,6 +500,14 @@
           <t>Arizona</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AZ</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>6731484</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -485,6 +518,14 @@
           <t>Arkansas</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2966369</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -495,6 +536,14 @@
           <t>California</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>38802500</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -505,6 +554,14 @@
           <t>Colorado</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5355866</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -515,6 +572,14 @@
           <t>Connecticut</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CT</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3596677</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -525,6 +590,14 @@
           <t>Delaware</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>935614</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -535,6 +608,14 @@
           <t>District of Columbia</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>658893</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -545,6 +626,14 @@
           <t>Florida</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>19893297</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -555,6 +644,14 @@
           <t>Georgia</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10097343</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -565,6 +662,14 @@
           <t>Hawaii</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>HI</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1419561</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -575,6 +680,14 @@
           <t>Idaho</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1634464</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -585,6 +698,14 @@
           <t>Illinois</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>12880580</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -595,6 +716,14 @@
           <t>Indiana</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>6596855</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -605,6 +734,14 @@
           <t>Iowa</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>3107126</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -615,6 +752,14 @@
           <t>Kansas</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>KS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2904021</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -625,6 +770,14 @@
           <t>Kentucky</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>KY</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4413457</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -635,6 +788,14 @@
           <t>Louisiana</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>LA</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4649676</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -645,6 +806,14 @@
           <t>Maine</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ME</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1330089</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -655,6 +824,14 @@
           <t>Maryland</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>MD</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5976407</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -665,6 +842,14 @@
           <t>Massachusetts</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>6745408</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -675,6 +860,14 @@
           <t>Michigan</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>9909877</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -685,6 +878,14 @@
           <t>Minnesota</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>MN</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>5457173</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -695,6 +896,14 @@
           <t>Mississippi</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2994079</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -705,6 +914,14 @@
           <t>Missouri</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>6063589</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -715,6 +932,14 @@
           <t>Montana</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1023579</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -725,6 +950,14 @@
           <t>Nebraska</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1881503</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -735,6 +968,14 @@
           <t>Nevada</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NV</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2839098</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -745,6 +986,14 @@
           <t>New Hampshire</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NH</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1326813</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -755,6 +1004,14 @@
           <t>New Jersey</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>NJ</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>8938175</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -765,6 +1022,14 @@
           <t>New Mexico</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>NM</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2085572</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -775,6 +1040,14 @@
           <t>New York</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>19746227</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -785,6 +1058,14 @@
           <t>North Carolina</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>9943964</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -795,6 +1076,14 @@
           <t>North Dakota</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>739482</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -805,6 +1094,14 @@
           <t>Ohio</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>OH</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>11594163</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -815,6 +1112,14 @@
           <t>Oklahoma</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>3878051</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -825,6 +1130,14 @@
           <t>Oregon</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>OR</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>3970239</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -835,6 +1148,14 @@
           <t>Pennsylvania</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>12787209</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -845,6 +1166,14 @@
           <t>Puerto Rico</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>3548397</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -855,6 +1184,14 @@
           <t>Rhode Island</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>RI</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1055173</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -865,6 +1202,14 @@
           <t>South Carolina</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>4832482</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -875,6 +1220,14 @@
           <t>South Dakota</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>853175</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -885,6 +1238,14 @@
           <t>Tennessee</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>TN</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>6549352</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -895,6 +1256,14 @@
           <t>Texas</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>26956958</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -905,6 +1274,14 @@
           <t>Utah</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>UT</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2942902</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -915,6 +1292,14 @@
           <t>Vermont</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>VT</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>626562</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -925,6 +1310,14 @@
           <t>Virginia</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>VA</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>8326289</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -935,6 +1328,14 @@
           <t>Washington</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>WA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>7061530</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -945,6 +1346,14 @@
           <t>West Virginia</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>WV</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>1850326</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -955,6 +1364,14 @@
           <t>Wisconsin</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>WI</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>5757564</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -965,555 +1382,12 @@
           <t>Wyoming</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Postal</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Population</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>4849377</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AK</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>736732</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>6731484</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AR</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2966369</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>38802500</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>CO</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5355866</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>CT</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>3596677</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>DE</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>935614</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>658893</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FL</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>19893297</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>10097343</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>HI</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1419561</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1634464</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>IL</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>12880580</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>6596855</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>IA</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>3107126</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>KS</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>2904021</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>KY</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>4413457</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>LA</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>4649676</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ME</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1330089</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MD</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>5976407</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>MA</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>6745408</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MI</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>9909877</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MN</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>5457173</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>2994079</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>MO</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>6063589</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>MT</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1023579</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>NE</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>1881503</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>NV</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>2839098</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>NH</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>1326813</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>NJ</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>8938175</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>NM</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>2085572</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>19746227</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>NC</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>9943964</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>739482</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>OH</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>11594163</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>3878051</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>OR</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>3970239</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>PA</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>12787209</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>PR</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>3548397</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>RI</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>1055173</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>4832482</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>SD</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>853175</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>TN</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>6549352</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>26956958</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>UT</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>2942902</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>VT</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>626562</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>VA</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>8326289</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>WA</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>7061530</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>WV</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>1850326</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>WI</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>5757564</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>WY</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="D53" t="n">
         <v>584153</v>
       </c>
     </row>

</xml_diff>